<commit_message>
some basic data for analysis
</commit_message>
<xml_diff>
--- a/experiment/results/results_raw.xlsx
+++ b/experiment/results/results_raw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="12240" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Natural" sheetId="1" r:id="rId1"/>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8267,408 +8267,6 @@
       </c>
       <c r="DE23" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:109">
-      <c r="A25">
-        <f>AVERAGE(A2:A23)</f>
-        <v>6.2272727272727275</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ref="B25:BM25" si="0">AVERAGE(B2:B23)</f>
-        <v>6.0454545454545459</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>6.7272727272727275</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>4.3636363636363633</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>3.7272727272727271</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>3.0454545454545454</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>4.8636363636363633</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>3.5909090909090908</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>8.3181818181818183</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
-        <v>7.0909090909090908</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="0"/>
-        <v>7.2272727272727275</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="0"/>
-        <v>3.7272727272727271</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="0"/>
-        <v>1.9090909090909092</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="0"/>
-        <v>4.7727272727272725</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="0"/>
-        <v>8.1363636363636367</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="0"/>
-        <v>7.8181818181818183</v>
-      </c>
-      <c r="T25">
-        <f t="shared" si="0"/>
-        <v>7.2727272727272725</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="0"/>
-        <v>8.3636363636363633</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="0"/>
-        <v>4.3181818181818183</v>
-      </c>
-      <c r="W25">
-        <f t="shared" si="0"/>
-        <v>7.1363636363636367</v>
-      </c>
-      <c r="X25">
-        <f t="shared" si="0"/>
-        <v>6.6363636363636367</v>
-      </c>
-      <c r="Y25">
-        <f t="shared" si="0"/>
-        <v>8.545454545454545</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="0"/>
-        <v>8.3636363636363633</v>
-      </c>
-      <c r="AA25">
-        <f t="shared" si="0"/>
-        <v>5.3636363636363633</v>
-      </c>
-      <c r="AB25">
-        <f t="shared" si="0"/>
-        <v>2.6363636363636362</v>
-      </c>
-      <c r="AC25">
-        <f t="shared" si="0"/>
-        <v>5.9545454545454541</v>
-      </c>
-      <c r="AD25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AE25">
-        <f t="shared" si="0"/>
-        <v>5.4545454545454541</v>
-      </c>
-      <c r="AF25">
-        <f t="shared" si="0"/>
-        <v>7.5909090909090908</v>
-      </c>
-      <c r="AG25">
-        <f t="shared" si="0"/>
-        <v>8.454545454545455</v>
-      </c>
-      <c r="AH25">
-        <f t="shared" si="0"/>
-        <v>6.9090909090909092</v>
-      </c>
-      <c r="AI25">
-        <f t="shared" si="0"/>
-        <v>2.9545454545454546</v>
-      </c>
-      <c r="AJ25">
-        <f t="shared" si="0"/>
-        <v>7.3636363636363633</v>
-      </c>
-      <c r="AK25">
-        <f t="shared" si="0"/>
-        <v>8.6363636363636367</v>
-      </c>
-      <c r="AL25">
-        <f t="shared" si="0"/>
-        <v>8.5909090909090917</v>
-      </c>
-      <c r="AM25">
-        <f t="shared" si="0"/>
-        <v>7.3636363636363633</v>
-      </c>
-      <c r="AN25">
-        <f t="shared" si="0"/>
-        <v>8.8636363636363633</v>
-      </c>
-      <c r="AO25">
-        <f t="shared" si="0"/>
-        <v>4.1818181818181817</v>
-      </c>
-      <c r="AP25">
-        <f t="shared" si="0"/>
-        <v>3.7272727272727271</v>
-      </c>
-      <c r="AQ25">
-        <f t="shared" si="0"/>
-        <v>4.7272727272727275</v>
-      </c>
-      <c r="AR25">
-        <f t="shared" si="0"/>
-        <v>4.0909090909090908</v>
-      </c>
-      <c r="AS25">
-        <f t="shared" si="0"/>
-        <v>3.4090909090909092</v>
-      </c>
-      <c r="AT25">
-        <f t="shared" si="0"/>
-        <v>5.8181818181818183</v>
-      </c>
-      <c r="AU25">
-        <f t="shared" si="0"/>
-        <v>5.4090909090909092</v>
-      </c>
-      <c r="AV25">
-        <f t="shared" si="0"/>
-        <v>4.0454545454545459</v>
-      </c>
-      <c r="AW25">
-        <f t="shared" si="0"/>
-        <v>2.9090909090909092</v>
-      </c>
-      <c r="AX25">
-        <f t="shared" si="0"/>
-        <v>3.8181818181818183</v>
-      </c>
-      <c r="AY25">
-        <f t="shared" si="0"/>
-        <v>4.2727272727272725</v>
-      </c>
-      <c r="AZ25">
-        <f t="shared" si="0"/>
-        <v>3.9090909090909092</v>
-      </c>
-      <c r="BA25">
-        <f t="shared" si="0"/>
-        <v>8.8181818181818183</v>
-      </c>
-      <c r="BB25">
-        <f t="shared" si="0"/>
-        <v>8.6818181818181817</v>
-      </c>
-      <c r="BC25">
-        <f t="shared" si="0"/>
-        <v>7.7727272727272725</v>
-      </c>
-      <c r="BD25">
-        <f t="shared" si="0"/>
-        <v>3.2272727272727271</v>
-      </c>
-      <c r="BE25">
-        <f t="shared" si="0"/>
-        <v>8.7272727272727266</v>
-      </c>
-      <c r="BF25">
-        <f t="shared" si="0"/>
-        <v>6.8181818181818183</v>
-      </c>
-      <c r="BG25">
-        <f t="shared" si="0"/>
-        <v>7.8636363636363633</v>
-      </c>
-      <c r="BH25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="BI25">
-        <f t="shared" si="0"/>
-        <v>7.1818181818181817</v>
-      </c>
-      <c r="BJ25">
-        <f t="shared" si="0"/>
-        <v>7.9545454545454541</v>
-      </c>
-      <c r="BK25">
-        <f t="shared" si="0"/>
-        <v>7.3636363636363633</v>
-      </c>
-      <c r="BL25">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="BM25">
-        <f t="shared" si="0"/>
-        <v>3.5454545454545454</v>
-      </c>
-      <c r="BN25">
-        <f t="shared" ref="BN25:CV25" si="1">AVERAGE(BN2:BN23)</f>
-        <v>8.454545454545455</v>
-      </c>
-      <c r="BO25">
-        <f t="shared" si="1"/>
-        <v>4.4545454545454541</v>
-      </c>
-      <c r="BP25">
-        <f t="shared" si="1"/>
-        <v>8.954545454545455</v>
-      </c>
-      <c r="BQ25">
-        <f t="shared" si="1"/>
-        <v>8.8181818181818183</v>
-      </c>
-      <c r="BR25">
-        <f t="shared" si="1"/>
-        <v>8.954545454545455</v>
-      </c>
-      <c r="BS25">
-        <f t="shared" si="1"/>
-        <v>8.8636363636363633</v>
-      </c>
-      <c r="BT25">
-        <f t="shared" si="1"/>
-        <v>7.8636363636363633</v>
-      </c>
-      <c r="BU25">
-        <f t="shared" si="1"/>
-        <v>8.5909090909090917</v>
-      </c>
-      <c r="BV25">
-        <f t="shared" si="1"/>
-        <v>7.1818181818181817</v>
-      </c>
-      <c r="BW25">
-        <f t="shared" si="1"/>
-        <v>8.4090909090909083</v>
-      </c>
-      <c r="BX25">
-        <f t="shared" si="1"/>
-        <v>7.1818181818181817</v>
-      </c>
-      <c r="BY25">
-        <f t="shared" si="1"/>
-        <v>5.6818181818181817</v>
-      </c>
-      <c r="BZ25">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="CA25">
-        <f t="shared" si="1"/>
-        <v>8.6363636363636367</v>
-      </c>
-      <c r="CB25">
-        <f t="shared" si="1"/>
-        <v>8.454545454545455</v>
-      </c>
-      <c r="CC25">
-        <f t="shared" si="1"/>
-        <v>7.3636363636363633</v>
-      </c>
-      <c r="CD25">
-        <f t="shared" si="1"/>
-        <v>8.0909090909090917</v>
-      </c>
-      <c r="CE25">
-        <f t="shared" si="1"/>
-        <v>2.2272727272727271</v>
-      </c>
-      <c r="CF25">
-        <f t="shared" si="1"/>
-        <v>7.5909090909090908</v>
-      </c>
-      <c r="CG25">
-        <f t="shared" si="1"/>
-        <v>4.5454545454545459</v>
-      </c>
-      <c r="CH25">
-        <f t="shared" si="1"/>
-        <v>8.1818181818181817</v>
-      </c>
-      <c r="CI25">
-        <f t="shared" si="1"/>
-        <v>8.6818181818181817</v>
-      </c>
-      <c r="CJ25">
-        <f t="shared" si="1"/>
-        <v>8.4090909090909083</v>
-      </c>
-      <c r="CK25">
-        <f t="shared" si="1"/>
-        <v>8.8181818181818183</v>
-      </c>
-      <c r="CL25">
-        <f t="shared" si="1"/>
-        <v>7.9090909090909092</v>
-      </c>
-      <c r="CM25">
-        <f t="shared" si="1"/>
-        <v>8.6363636363636367</v>
-      </c>
-      <c r="CN25">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="CO25">
-        <f t="shared" si="1"/>
-        <v>8.3181818181818183</v>
-      </c>
-      <c r="CP25">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="CQ25">
-        <f t="shared" si="1"/>
-        <v>8.8181818181818183</v>
-      </c>
-      <c r="CR25">
-        <f t="shared" si="1"/>
-        <v>8.5909090909090917</v>
-      </c>
-      <c r="CS25">
-        <f t="shared" si="1"/>
-        <v>4.6363636363636367</v>
-      </c>
-      <c r="CT25">
-        <f t="shared" si="1"/>
-        <v>5.0454545454545459</v>
-      </c>
-      <c r="CU25">
-        <f t="shared" si="1"/>
-        <v>8.954545454545455</v>
-      </c>
-      <c r="CV25">
-        <f t="shared" si="1"/>
-        <v>8.454545454545455</v>
       </c>
     </row>
     <row r="44" spans="5:5">
@@ -8690,10 +8288,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DE29"/>
+  <dimension ref="A1:DE26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17055,408 +16653,6 @@
       </c>
       <c r="DE26" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:109">
-      <c r="A29">
-        <f>AVERAGE(A2:A26)</f>
-        <v>6.12</v>
-      </c>
-      <c r="B29">
-        <f t="shared" ref="B29:BM29" si="0">AVERAGE(B2:B26)</f>
-        <v>5.52</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>7.04</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>4.76</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>3.84</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>2.76</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>5.24</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>2.96</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="0"/>
-        <v>8.44</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>6.76</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="0"/>
-        <v>6.56</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="0"/>
-        <v>2.68</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>6.64</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="0"/>
-        <v>4.68</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="0"/>
-        <v>7.6</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="0"/>
-        <v>7.56</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="0"/>
-        <v>7.04</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="0"/>
-        <v>7.88</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="W29">
-        <f t="shared" si="0"/>
-        <v>7.44</v>
-      </c>
-      <c r="X29">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-      <c r="Y29">
-        <f t="shared" si="0"/>
-        <v>8.64</v>
-      </c>
-      <c r="Z29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AA29">
-        <f t="shared" si="0"/>
-        <v>5.48</v>
-      </c>
-      <c r="AB29">
-        <f t="shared" si="0"/>
-        <v>2.44</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="0"/>
-        <v>6.84</v>
-      </c>
-      <c r="AD29">
-        <f t="shared" si="0"/>
-        <v>2.08</v>
-      </c>
-      <c r="AE29">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="AF29">
-        <f t="shared" si="0"/>
-        <v>7.08</v>
-      </c>
-      <c r="AG29">
-        <f t="shared" si="0"/>
-        <v>8.36</v>
-      </c>
-      <c r="AH29">
-        <f t="shared" si="0"/>
-        <v>7.24</v>
-      </c>
-      <c r="AI29">
-        <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="AJ29">
-        <f t="shared" si="0"/>
-        <v>6.88</v>
-      </c>
-      <c r="AK29">
-        <f t="shared" si="0"/>
-        <v>8.6</v>
-      </c>
-      <c r="AL29">
-        <f t="shared" si="0"/>
-        <v>8.32</v>
-      </c>
-      <c r="AM29">
-        <f t="shared" si="0"/>
-        <v>6.72</v>
-      </c>
-      <c r="AN29">
-        <f t="shared" si="0"/>
-        <v>8.6</v>
-      </c>
-      <c r="AO29">
-        <f t="shared" si="0"/>
-        <v>4.72</v>
-      </c>
-      <c r="AP29">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="AQ29">
-        <f t="shared" si="0"/>
-        <v>3.52</v>
-      </c>
-      <c r="AR29">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AS29">
-        <f t="shared" si="0"/>
-        <v>3.28</v>
-      </c>
-      <c r="AT29">
-        <f t="shared" si="0"/>
-        <v>6.68</v>
-      </c>
-      <c r="AU29">
-        <f t="shared" si="0"/>
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="AV29">
-        <f t="shared" si="0"/>
-        <v>3.56</v>
-      </c>
-      <c r="AW29">
-        <f t="shared" si="0"/>
-        <v>2.52</v>
-      </c>
-      <c r="AX29">
-        <f t="shared" si="0"/>
-        <v>5.08</v>
-      </c>
-      <c r="AY29">
-        <f t="shared" si="0"/>
-        <v>4.32</v>
-      </c>
-      <c r="AZ29">
-        <f t="shared" si="0"/>
-        <v>2.68</v>
-      </c>
-      <c r="BA29">
-        <f t="shared" si="0"/>
-        <v>8.68</v>
-      </c>
-      <c r="BB29">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-      <c r="BC29">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-      <c r="BD29">
-        <f t="shared" si="0"/>
-        <v>2.76</v>
-      </c>
-      <c r="BE29">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-      <c r="BF29">
-        <f t="shared" si="0"/>
-        <v>6.48</v>
-      </c>
-      <c r="BG29">
-        <f t="shared" si="0"/>
-        <v>7.84</v>
-      </c>
-      <c r="BH29">
-        <f t="shared" si="0"/>
-        <v>8.24</v>
-      </c>
-      <c r="BI29">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-      <c r="BJ29">
-        <f t="shared" si="0"/>
-        <v>7.84</v>
-      </c>
-      <c r="BK29">
-        <f t="shared" si="0"/>
-        <v>7.08</v>
-      </c>
-      <c r="BL29">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-      <c r="BM29">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="BN29">
-        <f t="shared" ref="BN29:CV29" si="1">AVERAGE(BN2:BN26)</f>
-        <v>8.4</v>
-      </c>
-      <c r="BO29">
-        <f t="shared" si="1"/>
-        <v>3.76</v>
-      </c>
-      <c r="BP29">
-        <f t="shared" si="1"/>
-        <v>8.6</v>
-      </c>
-      <c r="BQ29">
-        <f t="shared" si="1"/>
-        <v>8.76</v>
-      </c>
-      <c r="BR29">
-        <f t="shared" si="1"/>
-        <v>8.76</v>
-      </c>
-      <c r="BS29">
-        <f t="shared" si="1"/>
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="BT29">
-        <f t="shared" si="1"/>
-        <v>8.08</v>
-      </c>
-      <c r="BU29">
-        <f t="shared" si="1"/>
-        <v>8.44</v>
-      </c>
-      <c r="BV29">
-        <f t="shared" si="1"/>
-        <v>6.84</v>
-      </c>
-      <c r="BW29">
-        <f t="shared" si="1"/>
-        <v>8.48</v>
-      </c>
-      <c r="BX29">
-        <f t="shared" si="1"/>
-        <v>6.44</v>
-      </c>
-      <c r="BY29">
-        <f t="shared" si="1"/>
-        <v>6.08</v>
-      </c>
-      <c r="BZ29">
-        <f t="shared" si="1"/>
-        <v>8.76</v>
-      </c>
-      <c r="CA29">
-        <f t="shared" si="1"/>
-        <v>7.76</v>
-      </c>
-      <c r="CB29">
-        <f t="shared" si="1"/>
-        <v>8.6</v>
-      </c>
-      <c r="CC29">
-        <f t="shared" si="1"/>
-        <v>7.12</v>
-      </c>
-      <c r="CD29">
-        <f t="shared" si="1"/>
-        <v>8.08</v>
-      </c>
-      <c r="CE29">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="CF29">
-        <f t="shared" si="1"/>
-        <v>7.84</v>
-      </c>
-      <c r="CG29">
-        <f t="shared" si="1"/>
-        <v>4.12</v>
-      </c>
-      <c r="CH29">
-        <f t="shared" si="1"/>
-        <v>8.52</v>
-      </c>
-      <c r="CI29">
-        <f t="shared" si="1"/>
-        <v>8.64</v>
-      </c>
-      <c r="CJ29">
-        <f t="shared" si="1"/>
-        <v>8.48</v>
-      </c>
-      <c r="CK29">
-        <f t="shared" si="1"/>
-        <v>8.64</v>
-      </c>
-      <c r="CL29">
-        <f t="shared" si="1"/>
-        <v>8.64</v>
-      </c>
-      <c r="CM29">
-        <f t="shared" si="1"/>
-        <v>8.64</v>
-      </c>
-      <c r="CN29">
-        <f t="shared" si="1"/>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="CO29">
-        <f t="shared" si="1"/>
-        <v>8.32</v>
-      </c>
-      <c r="CP29">
-        <f t="shared" si="1"/>
-        <v>8.68</v>
-      </c>
-      <c r="CQ29">
-        <f t="shared" si="1"/>
-        <v>8.56</v>
-      </c>
-      <c r="CR29">
-        <f t="shared" si="1"/>
-        <v>8.48</v>
-      </c>
-      <c r="CS29">
-        <f t="shared" si="1"/>
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="CT29">
-        <f t="shared" si="1"/>
-        <v>4.32</v>
-      </c>
-      <c r="CU29">
-        <f t="shared" si="1"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="CV29">
-        <f t="shared" si="1"/>
-        <v>8.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>